<commit_message>
DDTFE - getting data and filling it into arrayList
</commit_message>
<xml_diff>
--- a/dantests/exceltests.xlsx
+++ b/dantests/exceltests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danier Javid\Desktop\Courses\selenium\dantests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A3D815-D41A-43AB-80EC-3B59EDA5A838}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDEB84C-49AB-4BBB-85F6-9075C70C8D14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="2460" windowWidth="15375" windowHeight="7875" xr2:uid="{1E372683-4BAF-4A2B-BDBD-B972A807C2F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1E372683-4BAF-4A2B-BDBD-B972A807C2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +89,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,8 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,89 +450,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7108253B-A1E5-4D79-B636-6A7D77DAF23E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>21</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>200</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>